<commit_message>
updated divisions for last season
</commit_message>
<xml_diff>
--- a/LeagueTable.xlsx
+++ b/LeagueTable.xlsx
@@ -938,54 +938,54 @@
     <t>Hartlepool</t>
   </si>
   <si>
+    <t>Bromley</t>
+  </si>
+  <si>
+    <t>Wrexham</t>
+  </si>
+  <si>
     <t>Notts County</t>
   </si>
   <si>
-    <t>Wrexham</t>
-  </si>
-  <si>
-    <t>Bromley</t>
-  </si>
-  <si>
     <t>Chesterfield</t>
   </si>
   <si>
+    <t>Solihull</t>
+  </si>
+  <si>
     <t>Eastleigh</t>
   </si>
   <si>
     <t>Halifax</t>
   </si>
   <si>
-    <t>Solihull</t>
-  </si>
-  <si>
     <t>Dag and Red</t>
   </si>
   <si>
     <t>Boreham Wood</t>
   </si>
   <si>
+    <t>Maidenhead</t>
+  </si>
+  <si>
+    <t>Aldershot</t>
+  </si>
+  <si>
     <t>Yeovil</t>
   </si>
   <si>
-    <t>Aldershot</t>
-  </si>
-  <si>
-    <t>Maidenhead</t>
-  </si>
-  <si>
     <t>Altrincham</t>
   </si>
   <si>
     <t>Weymouth</t>
   </si>
   <si>
+    <t>Wealdstone</t>
+  </si>
+  <si>
     <t>Woking</t>
   </si>
   <si>
-    <t>Wealdstone</t>
-  </si>
-  <si>
     <t>Kings Lynn</t>
   </si>
   <si>
@@ -995,16 +995,16 @@
     <t>Dover Athletic</t>
   </si>
   <si>
-    <t>94</t>
-  </si>
-  <si>
-    <t>-52</t>
+    <t>98</t>
+  </si>
+  <si>
+    <t>-50</t>
   </si>
   <si>
     <t>-46</t>
   </si>
   <si>
-    <t>-55</t>
+    <t>-53</t>
   </si>
   <si>
     <t>84</t>
@@ -1760,12 +1760,12 @@
     <t>Almeria</t>
   </si>
   <si>
+    <t>Leganes</t>
+  </si>
+  <si>
     <t>Girona</t>
   </si>
   <si>
-    <t>Leganes</t>
-  </si>
-  <si>
     <t>Vallecano</t>
   </si>
   <si>
@@ -1775,13 +1775,16 @@
     <t>Ponferradina</t>
   </si>
   <si>
+    <t>Las Palmas</t>
+  </si>
+  <si>
+    <t>Fuenlabrada</t>
+  </si>
+  <si>
     <t>Mirandes</t>
   </si>
   <si>
-    <t>Las Palmas</t>
-  </si>
-  <si>
-    <t>Fuenlabrada</t>
+    <t>Malaga</t>
   </si>
   <si>
     <t>Oviedo</t>
@@ -1790,7 +1793,7 @@
     <t>Tenerife</t>
   </si>
   <si>
-    <t>Malaga</t>
+    <t>Alcorcon</t>
   </si>
   <si>
     <t>Cartagena</t>
@@ -1799,16 +1802,13 @@
     <t>Zaragoza</t>
   </si>
   <si>
-    <t>Alcorcon</t>
+    <t>Lugo</t>
+  </si>
+  <si>
+    <t>Sabadell</t>
   </si>
   <si>
     <t>Logrones</t>
-  </si>
-  <si>
-    <t>Lugo</t>
-  </si>
-  <si>
-    <t>Sabadell</t>
   </si>
   <si>
     <t>Castellon</t>
@@ -9859,7 +9859,7 @@
         <v>572</v>
       </c>
       <c r="C2" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="D2" t="s">
         <v>47</v>
@@ -9868,16 +9868,16 @@
         <v>19</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G2" t="s">
         <v>153</v>
       </c>
       <c r="H2" t="s">
-        <v>156</v>
+        <v>119</v>
       </c>
       <c r="I2" t="s">
-        <v>60</v>
+        <v>87</v>
       </c>
       <c r="J2" t="s">
         <v>293</v>
@@ -9894,28 +9894,28 @@
         <v>573</v>
       </c>
       <c r="C3" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="D3" t="s">
         <v>47</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F3" t="s">
         <v>17</v>
       </c>
       <c r="G3" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="H3" t="s">
-        <v>65</v>
+        <v>119</v>
       </c>
       <c r="I3" t="s">
         <v>65</v>
       </c>
       <c r="J3" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="K3" t="n">
         <v>2.0</v>
@@ -9929,10 +9929,10 @@
         <v>574</v>
       </c>
       <c r="C4" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="D4" t="s">
-        <v>48</v>
+        <v>151</v>
       </c>
       <c r="E4" t="s">
         <v>19</v>
@@ -9941,16 +9941,16 @@
         <v>20</v>
       </c>
       <c r="G4" t="s">
-        <v>70</v>
+        <v>115</v>
       </c>
       <c r="H4" t="s">
         <v>63</v>
       </c>
       <c r="I4" t="s">
-        <v>49</v>
+        <v>151</v>
       </c>
       <c r="J4" t="s">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="K4" t="n">
         <v>3.0</v>
@@ -9964,10 +9964,10 @@
         <v>575</v>
       </c>
       <c r="C5" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="D5" t="s">
-        <v>48</v>
+        <v>151</v>
       </c>
       <c r="E5" t="s">
         <v>19</v>
@@ -9976,16 +9976,16 @@
         <v>20</v>
       </c>
       <c r="G5" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="H5" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="I5" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="J5" t="s">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="K5" t="n">
         <v>4.0</v>
@@ -9999,28 +9999,28 @@
         <v>576</v>
       </c>
       <c r="C6" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="D6" t="s">
         <v>48</v>
       </c>
       <c r="E6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F6" t="s">
         <v>20</v>
       </c>
       <c r="G6" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="H6" t="s">
-        <v>64</v>
+        <v>90</v>
       </c>
       <c r="I6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="J6" t="s">
-        <v>71</v>
+        <v>153</v>
       </c>
       <c r="K6" t="n">
         <v>5.0</v>
@@ -10034,7 +10034,7 @@
         <v>577</v>
       </c>
       <c r="C7" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="D7" t="s">
         <v>49</v>
@@ -10043,16 +10043,16 @@
         <v>19</v>
       </c>
       <c r="F7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G7" t="s">
         <v>55</v>
       </c>
       <c r="H7" t="s">
-        <v>88</v>
+        <v>63</v>
       </c>
       <c r="I7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J7" t="s">
         <v>53</v>
@@ -10069,7 +10069,7 @@
         <v>578</v>
       </c>
       <c r="C8" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="D8" t="s">
         <v>26</v>
@@ -10078,16 +10078,16 @@
         <v>23</v>
       </c>
       <c r="F8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G8" t="s">
         <v>117</v>
       </c>
       <c r="H8" t="s">
-        <v>65</v>
+        <v>119</v>
       </c>
       <c r="I8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J8" t="s">
         <v>127</v>
@@ -10104,28 +10104,28 @@
         <v>579</v>
       </c>
       <c r="C9" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="D9" t="s">
         <v>24</v>
       </c>
       <c r="E9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F9" t="s">
         <v>24</v>
       </c>
       <c r="G9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H9" t="s">
-        <v>66</v>
+        <v>85</v>
       </c>
       <c r="I9" t="s">
         <v>76</v>
       </c>
       <c r="J9" t="s">
-        <v>84</v>
+        <v>51</v>
       </c>
       <c r="K9" t="n">
         <v>8.0</v>
@@ -10139,28 +10139,28 @@
         <v>580</v>
       </c>
       <c r="C10" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="D10" t="s">
         <v>23</v>
       </c>
       <c r="E10" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G10" t="s">
-        <v>89</v>
+        <v>61</v>
       </c>
       <c r="H10" t="s">
-        <v>88</v>
+        <v>59</v>
       </c>
       <c r="I10" t="s">
-        <v>190</v>
+        <v>223</v>
       </c>
       <c r="J10" t="s">
-        <v>57</v>
+        <v>84</v>
       </c>
       <c r="K10" t="n">
         <v>9.0</v>
@@ -10174,28 +10174,28 @@
         <v>581</v>
       </c>
       <c r="C11" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="D11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E11" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="F11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G11" t="s">
         <v>86</v>
       </c>
       <c r="H11" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="I11" t="s">
-        <v>226</v>
+        <v>190</v>
       </c>
       <c r="J11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="K11" t="n">
         <v>10.0</v>
@@ -10209,28 +10209,28 @@
         <v>582</v>
       </c>
       <c r="C12" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G12" t="s">
+        <v>89</v>
+      </c>
+      <c r="H12" t="s">
         <v>62</v>
       </c>
-      <c r="D12" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" t="s">
-        <v>27</v>
-      </c>
-      <c r="F12" t="s">
-        <v>21</v>
-      </c>
-      <c r="G12" t="s">
-        <v>87</v>
-      </c>
-      <c r="H12" t="s">
-        <v>86</v>
-      </c>
       <c r="I12" t="s">
-        <v>121</v>
+        <v>78</v>
       </c>
       <c r="J12" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="K12" t="n">
         <v>11.0</v>
@@ -10244,28 +10244,28 @@
         <v>583</v>
       </c>
       <c r="C13" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="D13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" t="s">
         <v>20</v>
       </c>
-      <c r="E13" t="s">
-        <v>27</v>
-      </c>
       <c r="F13" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="G13" t="s">
-        <v>87</v>
+        <v>117</v>
       </c>
       <c r="H13" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="I13" t="s">
-        <v>190</v>
+        <v>374</v>
       </c>
       <c r="J13" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="K13" t="n">
         <v>12.0</v>
@@ -10279,28 +10279,28 @@
         <v>584</v>
       </c>
       <c r="C14" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="D14" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E14" t="s">
+        <v>49</v>
+      </c>
+      <c r="F14" t="s">
         <v>21</v>
       </c>
-      <c r="F14" t="s">
-        <v>25</v>
-      </c>
       <c r="G14" t="s">
-        <v>46</v>
+        <v>86</v>
       </c>
       <c r="H14" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="I14" t="s">
-        <v>73</v>
+        <v>190</v>
       </c>
       <c r="J14" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="K14" t="n">
         <v>13.0</v>
@@ -10314,28 +10314,28 @@
         <v>585</v>
       </c>
       <c r="C15" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="D15" t="s">
         <v>22</v>
       </c>
       <c r="E15" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G15" t="s">
-        <v>46</v>
+        <v>90</v>
       </c>
       <c r="H15" t="s">
-        <v>72</v>
+        <v>90</v>
       </c>
       <c r="I15" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="J15" t="s">
-        <v>85</v>
+        <v>55</v>
       </c>
       <c r="K15" t="n">
         <v>14.0</v>
@@ -10349,28 +10349,28 @@
         <v>586</v>
       </c>
       <c r="C16" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="D16" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F16" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="G16" t="s">
-        <v>87</v>
+        <v>64</v>
       </c>
       <c r="H16" t="s">
-        <v>52</v>
+        <v>88</v>
       </c>
       <c r="I16" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="J16" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="K16" t="n">
         <v>15.0</v>
@@ -10384,28 +10384,28 @@
         <v>587</v>
       </c>
       <c r="C17" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="D17" t="s">
         <v>21</v>
       </c>
       <c r="E17" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F17" t="s">
         <v>26</v>
       </c>
       <c r="G17" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="H17" t="s">
-        <v>89</v>
+        <v>55</v>
       </c>
       <c r="I17" t="s">
-        <v>261</v>
+        <v>226</v>
       </c>
       <c r="J17" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="K17" t="n">
         <v>16.0</v>
@@ -10419,28 +10419,28 @@
         <v>588</v>
       </c>
       <c r="C18" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="D18" t="s">
         <v>21</v>
       </c>
       <c r="E18" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F18" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="G18" t="s">
-        <v>91</v>
+        <v>46</v>
       </c>
       <c r="H18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I18" t="s">
-        <v>226</v>
+        <v>158</v>
       </c>
       <c r="J18" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="K18" t="n">
         <v>17.0</v>
@@ -10454,28 +10454,28 @@
         <v>589</v>
       </c>
       <c r="C19" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="D19" t="s">
         <v>20</v>
       </c>
       <c r="E19" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F19" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="G19" t="s">
-        <v>119</v>
+        <v>89</v>
       </c>
       <c r="H19" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="I19" t="s">
-        <v>225</v>
+        <v>375</v>
       </c>
       <c r="J19" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="K19" t="n">
         <v>18.0</v>
@@ -10489,28 +10489,28 @@
         <v>590</v>
       </c>
       <c r="C20" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="D20" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F20" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G20" t="s">
-        <v>117</v>
+        <v>63</v>
       </c>
       <c r="H20" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="I20" t="s">
-        <v>75</v>
+        <v>226</v>
       </c>
       <c r="J20" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="K20" t="n">
         <v>19.0</v>
@@ -10524,28 +10524,28 @@
         <v>591</v>
       </c>
       <c r="C21" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="D21" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E21" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F21" t="s">
-        <v>27</v>
+        <v>48</v>
       </c>
       <c r="G21" t="s">
-        <v>89</v>
+        <v>119</v>
       </c>
       <c r="H21" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="I21" t="s">
-        <v>374</v>
+        <v>191</v>
       </c>
       <c r="J21" t="s">
-        <v>87</v>
+        <v>60</v>
       </c>
       <c r="K21" t="n">
         <v>20.0</v>
@@ -10559,7 +10559,7 @@
         <v>592</v>
       </c>
       <c r="C22" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="D22" t="s">
         <v>20</v>
@@ -10568,16 +10568,16 @@
         <v>17</v>
       </c>
       <c r="F22" t="s">
-        <v>157</v>
+        <v>189</v>
       </c>
       <c r="G22" t="s">
         <v>128</v>
       </c>
       <c r="H22" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="I22" t="s">
-        <v>75</v>
+        <v>159</v>
       </c>
       <c r="J22" t="s">
         <v>62</v>
@@ -10594,7 +10594,7 @@
         <v>593</v>
       </c>
       <c r="C23" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="D23" t="s">
         <v>18</v>
@@ -10603,16 +10603,16 @@
         <v>20</v>
       </c>
       <c r="F23" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="G23" t="s">
-        <v>120</v>
+        <v>155</v>
       </c>
       <c r="H23" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="I23" t="s">
-        <v>80</v>
+        <v>160</v>
       </c>
       <c r="J23" t="s">
         <v>89</v>
@@ -15536,7 +15536,7 @@
         <v>297</v>
       </c>
       <c r="C2" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="D2" t="s">
         <v>116</v>
@@ -15545,16 +15545,16 @@
         <v>18</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G2" t="s">
         <v>264</v>
       </c>
       <c r="H2" t="s">
-        <v>46</v>
+        <v>90</v>
       </c>
       <c r="I2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="J2" t="s">
         <v>324</v>
@@ -15571,13 +15571,13 @@
         <v>298</v>
       </c>
       <c r="C3" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="D3" t="s">
         <v>47</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F3" t="s">
         <v>17</v>
@@ -15592,7 +15592,7 @@
         <v>91</v>
       </c>
       <c r="J3" t="s">
-        <v>293</v>
+        <v>187</v>
       </c>
       <c r="K3" t="n">
         <v>2.0</v>
@@ -15606,10 +15606,10 @@
         <v>299</v>
       </c>
       <c r="C4" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="D4" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="E4" t="s">
         <v>23</v>
@@ -15618,16 +15618,16 @@
         <v>16</v>
       </c>
       <c r="G4" t="s">
-        <v>153</v>
+        <v>264</v>
       </c>
       <c r="H4" t="s">
         <v>64</v>
       </c>
       <c r="I4" t="s">
-        <v>88</v>
+        <v>63</v>
       </c>
       <c r="J4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="K4" t="n">
         <v>3.0</v>
@@ -15641,10 +15641,10 @@
         <v>300</v>
       </c>
       <c r="C5" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="D5" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="E5" t="s">
         <v>19</v>
@@ -15653,16 +15653,16 @@
         <v>19</v>
       </c>
       <c r="G5" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="H5" t="s">
         <v>87</v>
       </c>
       <c r="I5" t="s">
-        <v>49</v>
+        <v>189</v>
       </c>
       <c r="J5" t="s">
-        <v>50</v>
+        <v>82</v>
       </c>
       <c r="K5" t="n">
         <v>4.0</v>
@@ -15676,28 +15676,28 @@
         <v>301</v>
       </c>
       <c r="C6" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="D6" t="s">
         <v>48</v>
       </c>
       <c r="E6" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G6" t="s">
-        <v>163</v>
+        <v>53</v>
       </c>
       <c r="H6" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="I6" t="s">
-        <v>151</v>
+        <v>22</v>
       </c>
       <c r="J6" t="s">
-        <v>71</v>
+        <v>264</v>
       </c>
       <c r="K6" t="n">
         <v>5.0</v>
@@ -15711,28 +15711,28 @@
         <v>302</v>
       </c>
       <c r="C7" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="D7" t="s">
         <v>48</v>
       </c>
       <c r="E7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F7" t="s">
         <v>21</v>
       </c>
       <c r="G7" t="s">
-        <v>152</v>
+        <v>53</v>
       </c>
       <c r="H7" t="s">
-        <v>87</v>
+        <v>60</v>
       </c>
       <c r="I7" t="s">
         <v>189</v>
       </c>
       <c r="J7" t="s">
-        <v>71</v>
+        <v>153</v>
       </c>
       <c r="K7" t="n">
         <v>6.0</v>
@@ -15746,28 +15746,28 @@
         <v>303</v>
       </c>
       <c r="C8" t="s">
+        <v>87</v>
+      </c>
+      <c r="D8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" t="s">
+        <v>163</v>
+      </c>
+      <c r="H8" t="s">
         <v>67</v>
       </c>
-      <c r="D8" t="s">
-        <v>49</v>
-      </c>
-      <c r="E8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F8" t="s">
-        <v>20</v>
-      </c>
-      <c r="G8" t="s">
-        <v>152</v>
-      </c>
-      <c r="H8" t="s">
-        <v>57</v>
-      </c>
       <c r="I8" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="J8" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="K8" t="n">
         <v>7.0</v>
@@ -15781,10 +15781,10 @@
         <v>304</v>
       </c>
       <c r="C9" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="D9" t="s">
-        <v>48</v>
+        <v>151</v>
       </c>
       <c r="E9" t="s">
         <v>15</v>
@@ -15793,16 +15793,16 @@
         <v>24</v>
       </c>
       <c r="G9" t="s">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="H9" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="I9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="J9" t="s">
-        <v>152</v>
+        <v>69</v>
       </c>
       <c r="K9" t="n">
         <v>8.0</v>
@@ -15816,28 +15816,28 @@
         <v>305</v>
       </c>
       <c r="C10" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="D10" t="s">
-        <v>27</v>
+        <v>48</v>
       </c>
       <c r="E10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" t="s">
+        <v>83</v>
+      </c>
+      <c r="H10" t="s">
+        <v>66</v>
+      </c>
+      <c r="I10" t="s">
         <v>21</v>
       </c>
-      <c r="F10" t="s">
-        <v>21</v>
-      </c>
-      <c r="G10" t="s">
-        <v>52</v>
-      </c>
-      <c r="H10" t="s">
-        <v>62</v>
-      </c>
-      <c r="I10" t="s">
-        <v>19</v>
-      </c>
       <c r="J10" t="s">
-        <v>152</v>
+        <v>53</v>
       </c>
       <c r="K10" t="n">
         <v>9.0</v>
@@ -15851,28 +15851,28 @@
         <v>306</v>
       </c>
       <c r="C11" t="s">
-        <v>62</v>
+        <v>87</v>
       </c>
       <c r="D11" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="E11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" t="s">
+        <v>52</v>
+      </c>
+      <c r="H11" t="s">
+        <v>87</v>
+      </c>
+      <c r="I11" t="s">
         <v>17</v>
       </c>
-      <c r="F11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G11" t="s">
-        <v>163</v>
-      </c>
-      <c r="H11" t="s">
-        <v>55</v>
-      </c>
-      <c r="I11" t="s">
-        <v>19</v>
-      </c>
       <c r="J11" t="s">
-        <v>127</v>
+        <v>152</v>
       </c>
       <c r="K11" t="n">
         <v>10.0</v>
@@ -15892,22 +15892,22 @@
         <v>49</v>
       </c>
       <c r="E12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G12" t="s">
-        <v>58</v>
+        <v>154</v>
       </c>
       <c r="H12" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="I12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J12" t="s">
-        <v>68</v>
+        <v>127</v>
       </c>
       <c r="K12" t="n">
         <v>11.0</v>
@@ -15921,28 +15921,28 @@
         <v>308</v>
       </c>
       <c r="C13" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="D13" t="s">
         <v>27</v>
       </c>
       <c r="E13" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F13" t="s">
         <v>25</v>
       </c>
       <c r="G13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H13" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="I13" t="s">
         <v>15</v>
       </c>
       <c r="J13" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="K13" t="n">
         <v>12.0</v>
@@ -15956,7 +15956,7 @@
         <v>309</v>
       </c>
       <c r="C14" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="D14" t="s">
         <v>22</v>
@@ -15965,16 +15965,16 @@
         <v>26</v>
       </c>
       <c r="F14" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G14" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="H14" t="s">
-        <v>86</v>
+        <v>54</v>
       </c>
       <c r="I14" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="J14" t="s">
         <v>84</v>
@@ -15994,25 +15994,25 @@
         <v>67</v>
       </c>
       <c r="D15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" t="s">
         <v>25</v>
       </c>
-      <c r="E15" t="s">
-        <v>16</v>
-      </c>
-      <c r="F15" t="s">
-        <v>49</v>
-      </c>
       <c r="G15" t="s">
-        <v>115</v>
+        <v>163</v>
       </c>
       <c r="H15" t="s">
-        <v>188</v>
+        <v>83</v>
       </c>
       <c r="I15" t="s">
-        <v>223</v>
+        <v>11</v>
       </c>
       <c r="J15" t="s">
-        <v>56</v>
+        <v>84</v>
       </c>
       <c r="K15" t="n">
         <v>14.0</v>
@@ -16026,28 +16026,28 @@
         <v>311</v>
       </c>
       <c r="C16" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="D16" t="s">
         <v>25</v>
       </c>
       <c r="E16" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F16" t="s">
         <v>48</v>
       </c>
       <c r="G16" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="H16" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="I16" t="s">
         <v>121</v>
       </c>
       <c r="J16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K16" t="n">
         <v>15.0</v>
@@ -16061,28 +16061,28 @@
         <v>312</v>
       </c>
       <c r="C17" t="s">
-        <v>62</v>
+        <v>87</v>
       </c>
       <c r="D17" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E17" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="F17" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="G17" t="s">
-        <v>58</v>
+        <v>115</v>
       </c>
       <c r="H17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I17" t="s">
-        <v>190</v>
+        <v>226</v>
       </c>
       <c r="J17" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="K17" t="n">
         <v>16.0</v>
@@ -16096,13 +16096,13 @@
         <v>313</v>
       </c>
       <c r="C18" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="D18" t="s">
         <v>22</v>
       </c>
       <c r="E18" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F18" t="s">
         <v>49</v>
@@ -16117,7 +16117,7 @@
         <v>79</v>
       </c>
       <c r="J18" t="s">
-        <v>54</v>
+        <v>85</v>
       </c>
       <c r="K18" t="n">
         <v>17.0</v>
@@ -16131,7 +16131,7 @@
         <v>314</v>
       </c>
       <c r="C19" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="D19" t="s">
         <v>20</v>
@@ -16140,16 +16140,16 @@
         <v>15</v>
       </c>
       <c r="F19" t="s">
-        <v>47</v>
+        <v>116</v>
       </c>
       <c r="G19" t="s">
         <v>86</v>
       </c>
       <c r="H19" t="s">
-        <v>53</v>
+        <v>153</v>
       </c>
       <c r="I19" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J19" t="s">
         <v>88</v>
@@ -16169,25 +16169,25 @@
         <v>67</v>
       </c>
       <c r="D20" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E20" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F20" t="s">
-        <v>47</v>
+        <v>116</v>
       </c>
       <c r="G20" t="s">
-        <v>86</v>
+        <v>54</v>
       </c>
       <c r="H20" t="s">
-        <v>152</v>
+        <v>113</v>
       </c>
       <c r="I20" t="s">
-        <v>124</v>
+        <v>321</v>
       </c>
       <c r="J20" t="s">
-        <v>90</v>
+        <v>117</v>
       </c>
       <c r="K20" t="n">
         <v>19.0</v>
@@ -16201,28 +16201,28 @@
         <v>316</v>
       </c>
       <c r="C21" t="s">
-        <v>62</v>
+        <v>87</v>
       </c>
       <c r="D21" t="s">
         <v>18</v>
       </c>
       <c r="E21" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F21" t="s">
         <v>116</v>
       </c>
       <c r="G21" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="H21" t="s">
-        <v>228</v>
+        <v>71</v>
       </c>
       <c r="I21" t="s">
-        <v>321</v>
+        <v>160</v>
       </c>
       <c r="J21" t="s">
-        <v>46</v>
+        <v>90</v>
       </c>
       <c r="K21" t="n">
         <v>20.0</v>
@@ -16236,19 +16236,19 @@
         <v>317</v>
       </c>
       <c r="C22" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="D22" t="s">
         <v>17</v>
       </c>
       <c r="E22" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F22" t="s">
         <v>116</v>
       </c>
       <c r="G22" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="H22" t="s">
         <v>320</v>
@@ -16257,7 +16257,7 @@
         <v>322</v>
       </c>
       <c r="J22" t="s">
-        <v>129</v>
+        <v>46</v>
       </c>
       <c r="K22" t="n">
         <v>21.0</v>
@@ -16271,10 +16271,10 @@
         <v>318</v>
       </c>
       <c r="C23" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="D23" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E23" t="s">
         <v>16</v>
@@ -16283,7 +16283,7 @@
         <v>119</v>
       </c>
       <c r="G23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H23" t="s">
         <v>229</v>
@@ -16292,7 +16292,7 @@
         <v>323</v>
       </c>
       <c r="J23" t="s">
-        <v>119</v>
+        <v>91</v>
       </c>
       <c r="K23" t="n">
         <v>22.0</v>

</xml_diff>